<commit_message>
converted excel to object[]
</commit_message>
<xml_diff>
--- a/OpenErmApplication/TestData/OpenEmrTestData.xlsx
+++ b/OpenErmApplication/TestData/OpenEmrTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JiDi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\B-Mine\Company\Company\Zensoft\OpenErmApplication\OpenErmApplication\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Password</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>peter123</t>
+  </si>
+  <si>
+    <t>peter12</t>
+  </si>
+  <si>
+    <t>223frrr</t>
   </si>
 </sst>
 </file>
@@ -374,9 +380,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -428,6 +436,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel to object[] and connected to invalid,about test
</commit_message>
<xml_diff>
--- a/OpenErmApplication/TestData/OpenEmrTestData.xlsx
+++ b/OpenErmApplication/TestData/OpenEmrTestData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialData" sheetId="1" r:id="rId1"/>
+    <sheet name="CheckHeaderAndVersionData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Password</t>
   </si>
@@ -50,19 +51,37 @@
     <t>Invalid username or password</t>
   </si>
   <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>king123</t>
+  </si>
+  <si>
     <t>Danish</t>
   </si>
   <si>
-    <t>peter</t>
-  </si>
-  <si>
-    <t>peter123</t>
-  </si>
-  <si>
-    <t>peter12</t>
-  </si>
-  <si>
-    <t>223frrr</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>English (Indian)</t>
+  </si>
+  <si>
+    <t>Expected About Header</t>
+  </si>
+  <si>
+    <t>Expected Version</t>
+  </si>
+  <si>
+    <t>About OpenEMR</t>
+  </si>
+  <si>
+    <t>Version Number: v6.0.0 (2)</t>
+  </si>
+  <si>
+    <t>About OpenEMR787</t>
   </si>
 </sst>
 </file>
@@ -380,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,44 +443,89 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>